<commit_message>
Update on 20231212 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/Jobs/2021年3月31日前厂商离沪意向排摸(1).xlsx
+++ b/文档/其他文档/Others/Jobs/2021年3月31日前厂商离沪意向排摸(1).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>2021年3月31日前员工离沪意向排摸</t>
   </si>
@@ -44,26 +44,6 @@
   </si>
   <si>
     <t>备注</t>
-  </si>
-  <si>
-    <t>上海埃帕信息科技有限公司</t>
-  </si>
-  <si>
-    <t>沈健</t>
-  </si>
-  <si>
-    <t>留沪</t>
-  </si>
-  <si>
-    <t>上海市杨浦区武川路99弄101号405室</t>
-  </si>
-  <si>
-    <t>张轶晟</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>上海市黄浦区中山南路1711弄1号506室</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -71,7 +51,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -155,7 +135,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -164,7 +144,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -497,46 +477,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>15221582155</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>13918581983</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>